<commit_message>
input field data to soil pit data excel
</commit_message>
<xml_diff>
--- a/data/soilpit_data.xlsx
+++ b/data/soilpit_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sophia.EMMA\Documents\GitHub\hillslope-project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\HS_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CD938D-E351-499A-A711-DEF474423D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA474B05-53ED-4DF9-AB44-A15DC353C5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72" yWindow="0" windowWidth="11292" windowHeight="16560" xr2:uid="{128AE9C5-A4E0-44D6-AEE2-927BDFCAF568}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{128AE9C5-A4E0-44D6-AEE2-927BDFCAF568}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t>Location</t>
   </si>
@@ -123,16 +123,102 @@
   </si>
   <si>
     <t>LC3.steep.4</t>
+  </si>
+  <si>
+    <t>depth 1 (cm)</t>
+  </si>
+  <si>
+    <t>depth 2 (cm)</t>
+  </si>
+  <si>
+    <t>depth 3 (cm)</t>
+  </si>
+  <si>
+    <t>Hs1.1</t>
+  </si>
+  <si>
+    <t>Hs1.2</t>
+  </si>
+  <si>
+    <t>Hs1.1.1</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Hs1.1.2</t>
+  </si>
+  <si>
+    <t>Hs1.1.3</t>
+  </si>
+  <si>
+    <t>Bedding plane widths (cm)</t>
+  </si>
+  <si>
+    <t>Depth to saprolite</t>
+  </si>
+  <si>
+    <t>28, 10, 9, 30</t>
+  </si>
+  <si>
+    <t>10, 5, 35, 1, 5, 3, 18, 10, 9, 0.5</t>
+  </si>
+  <si>
+    <t>Depth to Bedrock (cm)</t>
+  </si>
+  <si>
+    <t>greater than 80, topped by 23, 40, 30</t>
+  </si>
+  <si>
+    <t>no saprolite</t>
+  </si>
+  <si>
+    <t>35, 5, 11</t>
+  </si>
+  <si>
+    <t>38 maybe greater</t>
+  </si>
+  <si>
+    <t>ONLY BEDROCK</t>
+  </si>
+  <si>
+    <t>6, 2, 3, 4</t>
+  </si>
+  <si>
+    <t>EXPOSED BEDROCK</t>
+  </si>
+  <si>
+    <t>12, 25, 22, 9, 8</t>
+  </si>
+  <si>
+    <t>HS1.1500.1</t>
+  </si>
+  <si>
+    <t>HS1.1500.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -146,10 +232,96 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -158,8 +330,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,201 +657,473 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4C229D-DDB1-496A-9716-7D4F09DB5DBD}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" customWidth="1"/>
-    <col min="5" max="5" width="36.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.44140625" customWidth="1"/>
+    <col min="10" max="10" width="36.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="9"/>
+      <c r="C1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C2">
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>32</v>
+      </c>
+      <c r="H3">
         <v>125.59</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C3">
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
+      <c r="H4">
         <v>91.38</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C4">
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>24</v>
+      </c>
+      <c r="H5">
         <v>51.07</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C5">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>40</v>
+      </c>
+      <c r="H6">
         <v>25.18</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C6">
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>16</v>
+      </c>
+      <c r="H7">
         <v>113.63</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C7">
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="H8">
         <v>69.83</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C8">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="H9">
         <v>46.29</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C9">
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10">
         <v>24.71</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C10">
+      <c r="B11">
+        <v>65</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="H11">
         <v>29.38</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C11">
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12">
         <v>61.99</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C12">
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="H13">
         <v>111.31</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C13">
+      <c r="H14">
         <v>194.47</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C14">
+      <c r="F15">
+        <v>28</v>
+      </c>
+      <c r="H15">
         <v>464.36</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C15">
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>34</v>
+      </c>
+      <c r="H16">
         <v>336.62</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C16">
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>24</v>
+      </c>
+      <c r="H17">
         <v>259.38</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18">
+        <v>9</v>
+      </c>
+      <c r="H18">
+        <v>227.07</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C17">
-        <v>227.07</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18">
+      <c r="H20">
         <v>185.16</v>
       </c>
     </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22">
+        <v>6.5</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23">
+        <v>37</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="F29">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31">
+        <v>25</v>
+      </c>
+      <c r="F31">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:E1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>